<commit_message>
Merged Landing and base into final.py
</commit_message>
<xml_diff>
--- a/scrapping/product_details.xlsx
+++ b/scrapping/product_details.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -451,7 +451,7 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Image URL</t>
+          <t>Image_URL</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
@@ -468,32 +468,32 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>EatNeat 12 Pc Knife Set: Colorful Non-Stick Coated Stainless Steel Knives, Protective Sheaths, Cutting Board, &amp; Sharpener - Gifts for New Home, Apartments, RV - Ergonomic Sharp Knives for Kitchen</t>
+          <t>['Stanley Quencher H2.0 FlowState Stainless Steel Vacuum Insulated Tumbler with Lid and Straw for Water, Iced Tea or Coffee']</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>4.7</t>
+          <t>['4.6']</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>$19.95</t>
+          <t>['$45.00']</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>https://m.media-amazon.com/images/I/715eSNI3G3L._AC_SX450_.jpg</t>
+          <t>['https://m.media-amazon.com/images/I/41Ewz2W3GPL._AC_SX425_.jpg']</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>About this itemComplete Chef's Collection: The EatNeat 12-Piece Knife Set features five stainless steel knives in vibrant colors, each with its own safety sheath, blending functionality with style, perfect for kitchen use and outdoor camping.All-in-One Preparation Tools: This set includes a sturdy cutting board and a precision sharpener, ensuring you're equipped for any slicing or chopping task, enhancing your home cooking experience.Space-Saving Design: Ideal for small kitchens and apartments, the set comes with a compact knife holder, offering a practical solution for organizing and storing your essential cooking tools neatly.Enhanced Safety and Durability: Each knife is accompanied by a color-coded safety sheath for easy identification and safe handling. The stainless steel construction is both durable and rust-resistant, ensuring long-lasting use.Versatile Cooking Accessories: Along with top-quality knives, sharpener and various cooking utensils, making it an indispensable kit for everyday culinary adventures and a practical addition to any cookware collection.</t>
+          <t>["About this itemYOUR DREAM TUMBLER: Whichever way your day flows, the H2.0 FlowState tumbler keeps you refreshed with fewer refills. Double wall vacuum insulation means drinks stay cold, iced or hot for hours. Choose between our 14oz, 20oz, 30oz,40oz and 64oz options depending on your hydration needs. The narrow base on all sizes (except 64oz) fits just about any car cup holder, keeping it right by your side.ADVANCED LID CONSTRUCTION: Whether you prefer small sips or maximum thirst quenching, Stanley has developed an advanced FlowState lid, featuring a rotating cover with three positions: a straw opening designed to resist splashes with a seal that holds the reusable straw in place, a drink opening, and a full-cover top for added leak resistance. We’ve also included an ergonomic, comfort-grip handle, so you can easily carry your ice-cold water to work, meetings, the gym or trips out of town.EARTH-FRIENDLY DURABILITY: Constructed of 90% recycled BPA free stainless steel for sustainable sipping, the Stanley Quencher H2.0 has the durability to stand up to a lifetime of use. Eliminate the use of single-use plastic bottles and straws with a travel tumbler built with sustainability in mind.DISHWASHER SAFE: Spend less time hunched over the sink and more time doing the things you love. Cleaning your tumbler and lid couldn't be easier, just pop them into the dishwasher. Unlike plastic bottles that retain stains &amp; smells, this metallic beauty comes out pristineLIFETIME WARRANTY: Since 1913 we’ve promised to provide rugged, capable gear for food and drink - accessories built to last a lifetime. It’s a promise we still keep. Stanley products purchased from Stanley Resellers come with a lifetime warranty. Rest easy knowing we’ve got your back through it all."]</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Quality, Sharpness, Color, Value, Size, Ease of use, Cover, Stain resistance</t>
+          <t>['Insulation, Color, Size, Appearance, Coldness, Quality, Value, Condition']</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Included different approach for progress shown during scrapping
</commit_message>
<xml_diff>
--- a/scrapping/product_details.xlsx
+++ b/scrapping/product_details.xlsx
@@ -468,32 +468,32 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>['Stanley Quencher H2.0 FlowState Stainless Steel Vacuum Insulated Tumbler with Lid and Straw for Water, Iced Tea or Coffee']</t>
+          <t>['BestOffice High-Back Gaming Chair PC Office Chair Computer Racing Chair PU Desk Task Chair Ergonomic Executive Swivel Rolling Chair with Lumbar Support for Back Pain Women, Men,White']</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>['4.6']</t>
+          <t>['4.4']</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>['$45.00']</t>
+          <t>['$89.99']</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>['https://m.media-amazon.com/images/I/41Ewz2W3GPL._AC_SX425_.jpg']</t>
+          <t>['https://m.media-amazon.com/images/I/61t4mpabO+L._AC_SY450_.jpg']</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>["About this itemYOUR DREAM TUMBLER: Whichever way your day flows, the H2.0 FlowState tumbler keeps you refreshed with fewer refills. Double wall vacuum insulation means drinks stay cold, iced or hot for hours. Choose between our 14oz, 20oz, 30oz,40oz and 64oz options depending on your hydration needs. The narrow base on all sizes (except 64oz) fits just about any car cup holder, keeping it right by your side.ADVANCED LID CONSTRUCTION: Whether you prefer small sips or maximum thirst quenching, Stanley has developed an advanced FlowState lid, featuring a rotating cover with three positions: a straw opening designed to resist splashes with a seal that holds the reusable straw in place, a drink opening, and a full-cover top for added leak resistance. We’ve also included an ergonomic, comfort-grip handle, so you can easily carry your ice-cold water to work, meetings, the gym or trips out of town.EARTH-FRIENDLY DURABILITY: Constructed of 90% recycled BPA free stainless steel for sustainable sipping, the Stanley Quencher H2.0 has the durability to stand up to a lifetime of use. Eliminate the use of single-use plastic bottles and straws with a travel tumbler built with sustainability in mind.DISHWASHER SAFE: Spend less time hunched over the sink and more time doing the things you love. Cleaning your tumbler and lid couldn't be easier, just pop them into the dishwasher. Unlike plastic bottles that retain stains &amp; smells, this metallic beauty comes out pristineLIFETIME WARRANTY: Since 1913 we’ve promised to provide rugged, capable gear for food and drink - accessories built to last a lifetime. It’s a promise we still keep. Stanley products purchased from Stanley Resellers come with a lifetime warranty. Rest easy knowing we’ve got your back through it all."]</t>
+          <t>['About this itemPu LeatherCOMFORT FROM EVERY ANGLE - Our high-back gaming chair is thickly cushioned for maximum comfort, whether you’re spending long hours at the office, in front of the computer, or gaming. Covered with breathable premium PU leather, the chair is equipped with freely adjustable lumbar support and a headrest pillow to protect your spine and neck, while the adjustable reclining feature allows users to lock in any reclining position, from 90-135°.MAXIMUM MOBILITY - Our chair are designed with long-lasting ergonomic construction, equipped with a BIFMA-certified heavy-duty metal base, providing stability and mobility with a 360° range of motion on smooth-rolling nylon casters so you can glide easily between work stations.EASY ASSEMBLY – Our chair comes ready to assemble, with all the hardware and necessary tools. With step-by-step instructions, you’ll be set up and ready to game, take on the office in about 10-15 minutes!CUSTOMER GUARANTEE – We want all of our customers to feel 100% satisfied, and ready to unwind from the comfort of our High-Back Office Chair. If you’re not satisfied, or have any questions, please contact BestOffice customer service.BUILT TO LAST - The high-back chair is built to endure, with a heavy-duty metal base, offering great stability and mobility for a capacity of up to 250 lbs.']</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>['Insulation, Color, Size, Appearance, Coldness, Quality, Value, Condition']</t>
+          <t>['Comfort, Ease of assembly, Value, Appearance, Quality, Support, Size, Reclining']</t>
         </is>
       </c>
     </row>

</xml_diff>